<commit_message>
Area Excel sheet delete columns
</commit_message>
<xml_diff>
--- a/area_data.xlsx
+++ b/area_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/niklas_winata_bwedu_de/Documents/Dokumente/GitHub/topic04_team02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fionasteinacker/Documents/GitHub/topic04_team02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DA9BB24-6832-4942-82D3-3E7B4295F57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234F1560-090D-F543-98FB-FB614A956552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{02B7231A-B9DA-4B72-B0B4-CBA124D3C133}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{02B7231A-B9DA-4B72-B0B4-CBA124D3C133}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -624,18 +624,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6B2F36-3548-4A62-8B1D-0C5A13EDF38B}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,19 +643,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1568737</v>
       </c>
-      <c r="C2">
-        <f>SUM(B2:B5,B60:B61)</f>
-        <v>7761662</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -663,7 +659,7 @@
         <v>1004092</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -671,7 +667,7 @@
         <v>622303</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -679,19 +675,15 @@
         <v>1525856</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2556640</v>
       </c>
-      <c r="C6">
-        <f>SUM(B6:B11)</f>
-        <v>16593475</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -699,7 +691,7 @@
         <v>968372</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -707,7 +699,7 @@
         <v>6199753</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -715,7 +707,7 @@
         <v>822478</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -723,7 +715,7 @@
         <v>2469746</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -731,19 +723,15 @@
         <v>3576486</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>4363000</v>
       </c>
-      <c r="C12">
-        <f>SUM(B12:B19)</f>
-        <v>36502500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -751,7 +739,7 @@
         <v>3552000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -759,7 +747,7 @@
         <v>6338000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -767,7 +755,7 @@
         <v>2819000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -775,7 +763,7 @@
         <v>5351000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -783,7 +771,7 @@
         <v>4762362</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -791,7 +779,7 @@
         <v>2122000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -799,22 +787,15 @@
         <v>7195138</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>20493964</v>
       </c>
-      <c r="C20">
-        <f>SUM(B20:B39)</f>
-        <v>168855341</v>
-      </c>
-      <c r="D20">
-        <v>168855341</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -822,7 +803,7 @@
         <v>10322885</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -830,7 +811,7 @@
         <v>8124056</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -838,7 +819,7 @@
         <v>8839976</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -846,7 +827,7 @@
         <v>15744850</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -854,7 +835,7 @@
         <v>4161664</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -862,7 +843,7 @@
         <v>12778287</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -870,7 +851,7 @@
         <v>3161248</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -878,7 +859,7 @@
         <v>4305746</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -886,7 +867,7 @@
         <v>3859086</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -894,7 +875,7 @@
         <v>10885991</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -902,7 +883,7 @@
         <v>11730302</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -910,7 +891,7 @@
         <v>11424612</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -918,7 +899,7 @@
         <v>3026534</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -926,7 +907,7 @@
         <v>5291683</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -934,7 +915,7 @@
         <v>8299449</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -942,7 +923,7 @@
         <v>6946746</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -950,7 +931,7 @@
         <v>9605764</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -958,7 +939,7 @@
         <v>5512668</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -966,22 +947,15 @@
         <v>4339830</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40">
         <v>20107057</v>
       </c>
-      <c r="C40">
-        <f>SUM(B40:B56)</f>
-        <v>169644288</v>
-      </c>
-      <c r="D40">
-        <v>169644288</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -989,7 +963,7 @@
         <v>4505882</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -997,7 +971,7 @@
         <v>12533961</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1005,7 +979,7 @@
         <v>7838592</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1013,7 +987,7 @@
         <v>6538598</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1021,7 +995,7 @@
         <v>11472072</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1029,7 +1003,7 @@
         <v>6335060</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1037,7 +1011,7 @@
         <v>11678369</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1045,7 +1019,7 @@
         <v>12681259</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1053,7 +1027,7 @@
         <v>9597677</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1061,7 +1035,7 @@
         <v>6730246</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1069,7 +1043,7 @@
         <v>8607490</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1077,7 +1051,7 @@
         <v>16406650</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1085,7 +1059,7 @@
         <v>6596092</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1093,7 +1067,7 @@
         <v>10815854</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1101,7 +1075,7 @@
         <v>4531013</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1109,19 +1083,15 @@
         <v>12668416</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
       <c r="B57">
         <v>5196462</v>
       </c>
-      <c r="C57">
-        <f>SUM(B57:B59,B62:B64)</f>
-        <v>43047083</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1129,7 +1099,7 @@
         <v>19483148</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1137,7 +1107,7 @@
         <v>5358008</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1145,7 +1115,7 @@
         <v>2168327</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1153,7 +1123,7 @@
         <v>872347</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1161,7 +1131,7 @@
         <v>416707</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1169,7 +1139,7 @@
         <v>6225138</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1177,19 +1147,15 @@
         <v>6367620</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
       <c r="B65">
         <v>9942502</v>
       </c>
-      <c r="C65">
-        <f>SUM(B65:B78)</f>
-        <v>70715187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1197,7 +1163,7 @@
         <v>4708512</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1205,7 +1171,7 @@
         <v>4170895</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1213,7 +1179,7 @@
         <v>543034</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1221,7 +1187,7 @@
         <v>12891469</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1229,7 +1195,7 @@
         <v>3298045</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1237,7 +1203,7 @@
         <v>6009008</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1245,7 +1211,7 @@
         <v>7393889</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1253,7 +1219,7 @@
         <v>2478977</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1261,7 +1227,7 @@
         <v>4917519</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1269,7 +1235,7 @@
         <v>3424473</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1277,7 +1243,7 @@
         <v>1940356</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1285,7 +1251,7 @@
         <v>4521078</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>77</v>
       </c>

</xml_diff>